<commit_message>
add frcorerelated person 92e5d4123ea04d0f2e054aaa32578add1fb0775c
</commit_message>
<xml_diff>
--- a/395-flux---mise-à-jour-du-flux-1---projet-personnalisé/ig/StructureDefinition-tddui-bundle.xlsx
+++ b/395-flux---mise-à-jour-du-flux-1---projet-personnalisé/ig/StructureDefinition-tddui-bundle.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24594" uniqueCount="1024">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25734" uniqueCount="1062">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-12-18T09:45:01+00:00</t>
+    <t>2025-12-18T14:56:52+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -3131,6 +3131,121 @@
   </si>
   <si>
     <t>Bundle.entry:DUITaskPrestation.response.outcome</t>
+  </si>
+  <si>
+    <t>Bundle.entry:RelatedPerson</t>
+  </si>
+  <si>
+    <t>RelatedPerson</t>
+  </si>
+  <si>
+    <t>RelatedPerson conforming to the FrCoreRelatedPerson profile, used to convey information about a person related to the patient.</t>
+  </si>
+  <si>
+    <t>Bundle.entry:RelatedPerson.id</t>
+  </si>
+  <si>
+    <t>Bundle.entry:RelatedPerson.extension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:RelatedPerson.modifierExtension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:RelatedPerson.link</t>
+  </si>
+  <si>
+    <t>Bundle.entry:RelatedPerson.fullUrl</t>
+  </si>
+  <si>
+    <t>Bundle.entry:RelatedPerson.resource</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RelatedPerson {https://hl7.fr/ig/fhir/core/StructureDefinition/fr-core-related-person}
+</t>
+  </si>
+  <si>
+    <t>A person that is related to a patient, but who is not a direct target of care</t>
+  </si>
+  <si>
+    <t>Information about a person that is involved in the care for a patient, but who is not the target of healthcare, nor has a formal responsibility in the care process.</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>Bundle.entry:RelatedPerson.search</t>
+  </si>
+  <si>
+    <t>Bundle.entry:RelatedPerson.search.id</t>
+  </si>
+  <si>
+    <t>Bundle.entry:RelatedPerson.search.extension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:RelatedPerson.search.modifierExtension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:RelatedPerson.search.mode</t>
+  </si>
+  <si>
+    <t>Bundle.entry:RelatedPerson.search.score</t>
+  </si>
+  <si>
+    <t>Bundle.entry:RelatedPerson.request</t>
+  </si>
+  <si>
+    <t>Bundle.entry:RelatedPerson.request.id</t>
+  </si>
+  <si>
+    <t>Bundle.entry:RelatedPerson.request.extension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:RelatedPerson.request.modifierExtension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:RelatedPerson.request.method</t>
+  </si>
+  <si>
+    <t>Bundle.entry:RelatedPerson.request.url</t>
+  </si>
+  <si>
+    <t>Bundle.entry:RelatedPerson.request.ifNoneMatch</t>
+  </si>
+  <si>
+    <t>Bundle.entry:RelatedPerson.request.ifModifiedSince</t>
+  </si>
+  <si>
+    <t>Bundle.entry:RelatedPerson.request.ifMatch</t>
+  </si>
+  <si>
+    <t>Bundle.entry:RelatedPerson.request.ifNoneExist</t>
+  </si>
+  <si>
+    <t>Bundle.entry:RelatedPerson.response</t>
+  </si>
+  <si>
+    <t>Bundle.entry:RelatedPerson.response.id</t>
+  </si>
+  <si>
+    <t>Bundle.entry:RelatedPerson.response.extension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:RelatedPerson.response.modifierExtension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:RelatedPerson.response.status</t>
+  </si>
+  <si>
+    <t>Bundle.entry:RelatedPerson.response.location</t>
+  </si>
+  <si>
+    <t>Bundle.entry:RelatedPerson.response.etag</t>
+  </si>
+  <si>
+    <t>Bundle.entry:RelatedPerson.response.lastModified</t>
+  </si>
+  <si>
+    <t>Bundle.entry:RelatedPerson.response.outcome</t>
   </si>
   <si>
     <t>Bundle.signature</t>
@@ -3454,7 +3569,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AN689"/>
+  <dimension ref="A1:AN721"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -81445,9 +81560,11 @@
         <v>1018</v>
       </c>
       <c r="B689" t="s" s="2">
-        <v>1018</v>
-      </c>
-      <c r="C689" s="2"/>
+        <v>175</v>
+      </c>
+      <c r="C689" t="s" s="2">
+        <v>1019</v>
+      </c>
       <c r="D689" t="s" s="2">
         <v>77</v>
       </c>
@@ -81456,7 +81573,7 @@
         <v>78</v>
       </c>
       <c r="G689" t="s" s="2">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="H689" t="s" s="2">
         <v>77</v>
@@ -81468,20 +81585,16 @@
         <v>88</v>
       </c>
       <c r="K689" t="s" s="2">
-        <v>1019</v>
+        <v>145</v>
       </c>
       <c r="L689" t="s" s="2">
         <v>1020</v>
       </c>
       <c r="M689" t="s" s="2">
-        <v>1021</v>
-      </c>
-      <c r="N689" t="s" s="2">
-        <v>1022</v>
-      </c>
-      <c r="O689" t="s" s="2">
-        <v>1023</v>
-      </c>
+        <v>177</v>
+      </c>
+      <c r="N689" s="2"/>
+      <c r="O689" s="2"/>
       <c r="P689" t="s" s="2">
         <v>77</v>
       </c>
@@ -81529,30 +81642,3656 @@
         <v>77</v>
       </c>
       <c r="AF689" t="s" s="2">
-        <v>1018</v>
+        <v>175</v>
       </c>
       <c r="AG689" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH689" t="s" s="2">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="AI689" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AJ689" t="s" s="2">
+        <v>181</v>
+      </c>
+      <c r="AK689" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AL689" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AM689" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN689" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="s" s="2">
+        <v>1021</v>
+      </c>
+      <c r="B690" t="s" s="2">
+        <v>182</v>
+      </c>
+      <c r="C690" s="2"/>
+      <c r="D690" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="E690" s="2"/>
+      <c r="F690" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G690" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="H690" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I690" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="J690" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="K690" t="s" s="2">
+        <v>150</v>
+      </c>
+      <c r="L690" t="s" s="2">
+        <v>151</v>
+      </c>
+      <c r="M690" t="s" s="2">
+        <v>152</v>
+      </c>
+      <c r="N690" s="2"/>
+      <c r="O690" s="2"/>
+      <c r="P690" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q690" s="2"/>
+      <c r="R690" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="S690" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="T690" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="U690" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="V690" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="W690" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X690" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Y690" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Z690" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AA690" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB690" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AC690" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD690" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE690" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF690" t="s" s="2">
+        <v>153</v>
+      </c>
+      <c r="AG690" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH690" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AI690" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ690" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AK690" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AL690" t="s" s="2">
+        <v>154</v>
+      </c>
+      <c r="AM690" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN690" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="s" s="2">
+        <v>1022</v>
+      </c>
+      <c r="B691" t="s" s="2">
+        <v>183</v>
+      </c>
+      <c r="C691" s="2"/>
+      <c r="D691" t="s" s="2">
+        <v>156</v>
+      </c>
+      <c r="E691" s="2"/>
+      <c r="F691" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G691" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="H691" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I691" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="J691" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="K691" t="s" s="2">
+        <v>157</v>
+      </c>
+      <c r="L691" t="s" s="2">
+        <v>158</v>
+      </c>
+      <c r="M691" t="s" s="2">
+        <v>159</v>
+      </c>
+      <c r="N691" t="s" s="2">
+        <v>160</v>
+      </c>
+      <c r="O691" s="2"/>
+      <c r="P691" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q691" s="2"/>
+      <c r="R691" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="S691" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="T691" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="U691" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="V691" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="W691" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X691" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Y691" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Z691" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AA691" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB691" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AC691" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD691" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE691" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF691" t="s" s="2">
+        <v>161</v>
+      </c>
+      <c r="AG691" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH691" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AI691" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ691" t="s" s="2">
+        <v>162</v>
+      </c>
+      <c r="AK691" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AL691" t="s" s="2">
+        <v>154</v>
+      </c>
+      <c r="AM691" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN691" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="s" s="2">
+        <v>1023</v>
+      </c>
+      <c r="B692" t="s" s="2">
+        <v>184</v>
+      </c>
+      <c r="C692" s="2"/>
+      <c r="D692" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="E692" s="2"/>
+      <c r="F692" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G692" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="H692" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I692" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="J692" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="K692" t="s" s="2">
+        <v>157</v>
+      </c>
+      <c r="L692" t="s" s="2">
+        <v>165</v>
+      </c>
+      <c r="M692" t="s" s="2">
+        <v>166</v>
+      </c>
+      <c r="N692" t="s" s="2">
+        <v>160</v>
+      </c>
+      <c r="O692" t="s" s="2">
+        <v>167</v>
+      </c>
+      <c r="P692" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q692" s="2"/>
+      <c r="R692" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="S692" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="T692" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="U692" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="V692" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="W692" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X692" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Y692" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Z692" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AA692" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB692" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AC692" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD692" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE692" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF692" t="s" s="2">
+        <v>168</v>
+      </c>
+      <c r="AG692" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH692" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AI692" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ692" t="s" s="2">
+        <v>162</v>
+      </c>
+      <c r="AK692" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AL692" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AM692" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN692" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="s" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B693" t="s" s="2">
+        <v>185</v>
+      </c>
+      <c r="C693" s="2"/>
+      <c r="D693" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="E693" s="2"/>
+      <c r="F693" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G693" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="H693" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I693" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="J693" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="K693" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="L693" t="s" s="2">
+        <v>186</v>
+      </c>
+      <c r="M693" t="s" s="2">
+        <v>187</v>
+      </c>
+      <c r="N693" s="2"/>
+      <c r="O693" s="2"/>
+      <c r="P693" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q693" s="2"/>
+      <c r="R693" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="S693" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="T693" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="U693" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="V693" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="W693" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X693" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Y693" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Z693" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AA693" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB693" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AC693" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD693" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE693" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF693" t="s" s="2">
+        <v>185</v>
+      </c>
+      <c r="AG693" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH693" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AI693" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ693" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="AK689" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AL689" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM689" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN689" t="s" s="2">
+      <c r="AK693" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AL693" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AM693" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN693" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="s" s="2">
+        <v>1025</v>
+      </c>
+      <c r="B694" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="C694" s="2"/>
+      <c r="D694" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="E694" s="2"/>
+      <c r="F694" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G694" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="H694" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I694" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="J694" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="K694" t="s" s="2">
+        <v>101</v>
+      </c>
+      <c r="L694" t="s" s="2">
+        <v>189</v>
+      </c>
+      <c r="M694" t="s" s="2">
+        <v>190</v>
+      </c>
+      <c r="N694" t="s" s="2">
+        <v>191</v>
+      </c>
+      <c r="O694" s="2"/>
+      <c r="P694" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q694" s="2"/>
+      <c r="R694" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="S694" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="T694" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="U694" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="V694" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="W694" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X694" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Y694" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Z694" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AA694" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB694" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AC694" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD694" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE694" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF694" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="AG694" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH694" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AI694" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ694" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="AK694" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AL694" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AM694" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN694" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="s" s="2">
+        <v>1026</v>
+      </c>
+      <c r="B695" t="s" s="2">
+        <v>192</v>
+      </c>
+      <c r="C695" s="2"/>
+      <c r="D695" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="E695" s="2"/>
+      <c r="F695" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="G695" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="H695" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I695" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="J695" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="K695" t="s" s="2">
+        <v>1027</v>
+      </c>
+      <c r="L695" t="s" s="2">
+        <v>1028</v>
+      </c>
+      <c r="M695" t="s" s="2">
+        <v>1029</v>
+      </c>
+      <c r="N695" s="2"/>
+      <c r="O695" s="2"/>
+      <c r="P695" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q695" s="2"/>
+      <c r="R695" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="S695" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="T695" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="U695" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="V695" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="W695" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X695" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Y695" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Z695" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AA695" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB695" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AC695" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD695" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE695" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF695" t="s" s="2">
+        <v>192</v>
+      </c>
+      <c r="AG695" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH695" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AI695" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ695" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AK695" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AL695" t="s" s="2">
+        <v>1030</v>
+      </c>
+      <c r="AM695" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN695" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="s" s="2">
+        <v>1031</v>
+      </c>
+      <c r="B696" t="s" s="2">
+        <v>196</v>
+      </c>
+      <c r="C696" s="2"/>
+      <c r="D696" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="E696" s="2"/>
+      <c r="F696" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G696" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="H696" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I696" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="J696" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="K696" t="s" s="2">
+        <v>145</v>
+      </c>
+      <c r="L696" t="s" s="2">
+        <v>197</v>
+      </c>
+      <c r="M696" t="s" s="2">
+        <v>198</v>
+      </c>
+      <c r="N696" s="2"/>
+      <c r="O696" s="2"/>
+      <c r="P696" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q696" s="2"/>
+      <c r="R696" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="S696" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="T696" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="U696" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="V696" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="W696" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X696" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Y696" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Z696" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AA696" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB696" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AC696" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD696" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE696" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF696" t="s" s="2">
+        <v>196</v>
+      </c>
+      <c r="AG696" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH696" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AI696" t="s" s="2">
+        <v>199</v>
+      </c>
+      <c r="AJ696" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="AK696" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AL696" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AM696" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN696" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="s" s="2">
+        <v>1032</v>
+      </c>
+      <c r="B697" t="s" s="2">
+        <v>200</v>
+      </c>
+      <c r="C697" s="2"/>
+      <c r="D697" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="E697" s="2"/>
+      <c r="F697" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G697" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="H697" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I697" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="J697" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="K697" t="s" s="2">
+        <v>150</v>
+      </c>
+      <c r="L697" t="s" s="2">
+        <v>151</v>
+      </c>
+      <c r="M697" t="s" s="2">
+        <v>152</v>
+      </c>
+      <c r="N697" s="2"/>
+      <c r="O697" s="2"/>
+      <c r="P697" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q697" s="2"/>
+      <c r="R697" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="S697" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="T697" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="U697" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="V697" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="W697" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X697" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Y697" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Z697" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AA697" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB697" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AC697" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD697" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE697" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF697" t="s" s="2">
+        <v>153</v>
+      </c>
+      <c r="AG697" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH697" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AI697" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ697" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AK697" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AL697" t="s" s="2">
+        <v>154</v>
+      </c>
+      <c r="AM697" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN697" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="s" s="2">
+        <v>1033</v>
+      </c>
+      <c r="B698" t="s" s="2">
+        <v>201</v>
+      </c>
+      <c r="C698" s="2"/>
+      <c r="D698" t="s" s="2">
+        <v>156</v>
+      </c>
+      <c r="E698" s="2"/>
+      <c r="F698" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G698" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="H698" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I698" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="J698" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="K698" t="s" s="2">
+        <v>157</v>
+      </c>
+      <c r="L698" t="s" s="2">
+        <v>158</v>
+      </c>
+      <c r="M698" t="s" s="2">
+        <v>159</v>
+      </c>
+      <c r="N698" t="s" s="2">
+        <v>160</v>
+      </c>
+      <c r="O698" s="2"/>
+      <c r="P698" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q698" s="2"/>
+      <c r="R698" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="S698" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="T698" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="U698" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="V698" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="W698" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X698" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Y698" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Z698" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AA698" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB698" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AC698" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD698" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE698" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF698" t="s" s="2">
+        <v>161</v>
+      </c>
+      <c r="AG698" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH698" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AI698" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ698" t="s" s="2">
+        <v>162</v>
+      </c>
+      <c r="AK698" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AL698" t="s" s="2">
+        <v>154</v>
+      </c>
+      <c r="AM698" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN698" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="s" s="2">
+        <v>1034</v>
+      </c>
+      <c r="B699" t="s" s="2">
+        <v>202</v>
+      </c>
+      <c r="C699" s="2"/>
+      <c r="D699" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="E699" s="2"/>
+      <c r="F699" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G699" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="H699" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I699" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="J699" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="K699" t="s" s="2">
+        <v>157</v>
+      </c>
+      <c r="L699" t="s" s="2">
+        <v>165</v>
+      </c>
+      <c r="M699" t="s" s="2">
+        <v>166</v>
+      </c>
+      <c r="N699" t="s" s="2">
+        <v>160</v>
+      </c>
+      <c r="O699" t="s" s="2">
+        <v>167</v>
+      </c>
+      <c r="P699" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q699" s="2"/>
+      <c r="R699" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="S699" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="T699" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="U699" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="V699" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="W699" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X699" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Y699" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Z699" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AA699" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB699" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AC699" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD699" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE699" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF699" t="s" s="2">
+        <v>168</v>
+      </c>
+      <c r="AG699" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH699" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AI699" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ699" t="s" s="2">
+        <v>162</v>
+      </c>
+      <c r="AK699" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AL699" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AM699" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN699" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="s" s="2">
+        <v>1035</v>
+      </c>
+      <c r="B700" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="C700" s="2"/>
+      <c r="D700" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="E700" s="2"/>
+      <c r="F700" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G700" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="H700" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I700" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="J700" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="K700" t="s" s="2">
+        <v>107</v>
+      </c>
+      <c r="L700" t="s" s="2">
+        <v>204</v>
+      </c>
+      <c r="M700" t="s" s="2">
+        <v>205</v>
+      </c>
+      <c r="N700" t="s" s="2">
+        <v>206</v>
+      </c>
+      <c r="O700" s="2"/>
+      <c r="P700" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q700" s="2"/>
+      <c r="R700" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="S700" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="T700" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="U700" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="V700" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="W700" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X700" t="s" s="2">
+        <v>127</v>
+      </c>
+      <c r="Y700" t="s" s="2">
+        <v>207</v>
+      </c>
+      <c r="Z700" t="s" s="2">
+        <v>208</v>
+      </c>
+      <c r="AA700" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB700" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AC700" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD700" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE700" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF700" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="AG700" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH700" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AI700" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ700" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="AK700" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AL700" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AM700" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN700" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="s" s="2">
+        <v>1036</v>
+      </c>
+      <c r="B701" t="s" s="2">
+        <v>209</v>
+      </c>
+      <c r="C701" s="2"/>
+      <c r="D701" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="E701" s="2"/>
+      <c r="F701" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G701" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="H701" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I701" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="J701" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="K701" t="s" s="2">
+        <v>210</v>
+      </c>
+      <c r="L701" t="s" s="2">
+        <v>211</v>
+      </c>
+      <c r="M701" t="s" s="2">
+        <v>212</v>
+      </c>
+      <c r="N701" t="s" s="2">
+        <v>213</v>
+      </c>
+      <c r="O701" s="2"/>
+      <c r="P701" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q701" s="2"/>
+      <c r="R701" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="S701" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="T701" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="U701" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="V701" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="W701" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X701" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Y701" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Z701" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AA701" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB701" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AC701" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD701" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE701" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF701" t="s" s="2">
+        <v>209</v>
+      </c>
+      <c r="AG701" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH701" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AI701" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ701" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="AK701" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AL701" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AM701" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN701" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="s" s="2">
+        <v>1037</v>
+      </c>
+      <c r="B702" t="s" s="2">
+        <v>214</v>
+      </c>
+      <c r="C702" s="2"/>
+      <c r="D702" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="E702" s="2"/>
+      <c r="F702" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="G702" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="H702" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I702" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="J702" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="K702" t="s" s="2">
+        <v>145</v>
+      </c>
+      <c r="L702" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="M702" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="N702" s="2"/>
+      <c r="O702" s="2"/>
+      <c r="P702" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q702" s="2"/>
+      <c r="R702" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="S702" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="T702" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="U702" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="V702" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="W702" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X702" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Y702" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Z702" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AA702" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB702" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AC702" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD702" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE702" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF702" t="s" s="2">
+        <v>214</v>
+      </c>
+      <c r="AG702" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH702" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AI702" t="s" s="2">
+        <v>217</v>
+      </c>
+      <c r="AJ702" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="AK702" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AL702" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AM702" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN702" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="s" s="2">
+        <v>1038</v>
+      </c>
+      <c r="B703" t="s" s="2">
+        <v>218</v>
+      </c>
+      <c r="C703" s="2"/>
+      <c r="D703" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="E703" s="2"/>
+      <c r="F703" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G703" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="H703" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I703" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="J703" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="K703" t="s" s="2">
+        <v>150</v>
+      </c>
+      <c r="L703" t="s" s="2">
+        <v>151</v>
+      </c>
+      <c r="M703" t="s" s="2">
+        <v>152</v>
+      </c>
+      <c r="N703" s="2"/>
+      <c r="O703" s="2"/>
+      <c r="P703" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q703" s="2"/>
+      <c r="R703" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="S703" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="T703" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="U703" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="V703" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="W703" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X703" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Y703" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Z703" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AA703" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB703" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AC703" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD703" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE703" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF703" t="s" s="2">
+        <v>153</v>
+      </c>
+      <c r="AG703" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH703" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AI703" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ703" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AK703" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AL703" t="s" s="2">
+        <v>154</v>
+      </c>
+      <c r="AM703" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN703" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="s" s="2">
+        <v>1039</v>
+      </c>
+      <c r="B704" t="s" s="2">
+        <v>219</v>
+      </c>
+      <c r="C704" s="2"/>
+      <c r="D704" t="s" s="2">
+        <v>156</v>
+      </c>
+      <c r="E704" s="2"/>
+      <c r="F704" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G704" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="H704" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I704" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="J704" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="K704" t="s" s="2">
+        <v>157</v>
+      </c>
+      <c r="L704" t="s" s="2">
+        <v>158</v>
+      </c>
+      <c r="M704" t="s" s="2">
+        <v>159</v>
+      </c>
+      <c r="N704" t="s" s="2">
+        <v>160</v>
+      </c>
+      <c r="O704" s="2"/>
+      <c r="P704" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q704" s="2"/>
+      <c r="R704" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="S704" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="T704" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="U704" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="V704" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="W704" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X704" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Y704" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Z704" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AA704" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB704" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AC704" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD704" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE704" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF704" t="s" s="2">
+        <v>161</v>
+      </c>
+      <c r="AG704" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH704" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AI704" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ704" t="s" s="2">
+        <v>162</v>
+      </c>
+      <c r="AK704" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AL704" t="s" s="2">
+        <v>154</v>
+      </c>
+      <c r="AM704" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN704" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="s" s="2">
+        <v>1040</v>
+      </c>
+      <c r="B705" t="s" s="2">
+        <v>220</v>
+      </c>
+      <c r="C705" s="2"/>
+      <c r="D705" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="E705" s="2"/>
+      <c r="F705" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G705" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="H705" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I705" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="J705" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="K705" t="s" s="2">
+        <v>157</v>
+      </c>
+      <c r="L705" t="s" s="2">
+        <v>165</v>
+      </c>
+      <c r="M705" t="s" s="2">
+        <v>166</v>
+      </c>
+      <c r="N705" t="s" s="2">
+        <v>160</v>
+      </c>
+      <c r="O705" t="s" s="2">
+        <v>167</v>
+      </c>
+      <c r="P705" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q705" s="2"/>
+      <c r="R705" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="S705" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="T705" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="U705" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="V705" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="W705" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X705" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Y705" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Z705" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AA705" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB705" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AC705" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD705" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE705" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF705" t="s" s="2">
+        <v>168</v>
+      </c>
+      <c r="AG705" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH705" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AI705" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ705" t="s" s="2">
+        <v>162</v>
+      </c>
+      <c r="AK705" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AL705" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AM705" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN705" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="s" s="2">
+        <v>1041</v>
+      </c>
+      <c r="B706" t="s" s="2">
+        <v>221</v>
+      </c>
+      <c r="C706" s="2"/>
+      <c r="D706" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="E706" s="2"/>
+      <c r="F706" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="G706" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="H706" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I706" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="J706" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="K706" t="s" s="2">
+        <v>107</v>
+      </c>
+      <c r="L706" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="M706" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="N706" s="2"/>
+      <c r="O706" s="2"/>
+      <c r="P706" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q706" s="2"/>
+      <c r="R706" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="S706" t="s" s="2">
+        <v>292</v>
+      </c>
+      <c r="T706" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="U706" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="V706" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="W706" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X706" t="s" s="2">
+        <v>127</v>
+      </c>
+      <c r="Y706" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="Z706" t="s" s="2">
+        <v>225</v>
+      </c>
+      <c r="AA706" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB706" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AC706" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD706" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE706" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF706" t="s" s="2">
+        <v>221</v>
+      </c>
+      <c r="AG706" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AH706" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AI706" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ706" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="AK706" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AL706" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AM706" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN706" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="s" s="2">
+        <v>1042</v>
+      </c>
+      <c r="B707" t="s" s="2">
+        <v>226</v>
+      </c>
+      <c r="C707" s="2"/>
+      <c r="D707" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="E707" s="2"/>
+      <c r="F707" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="G707" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="H707" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I707" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="J707" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="K707" t="s" s="2">
+        <v>101</v>
+      </c>
+      <c r="L707" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="M707" t="s" s="2">
+        <v>228</v>
+      </c>
+      <c r="N707" t="s" s="2">
+        <v>229</v>
+      </c>
+      <c r="O707" s="2"/>
+      <c r="P707" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q707" s="2"/>
+      <c r="R707" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="S707" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="T707" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="U707" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="V707" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="W707" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X707" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Y707" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Z707" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AA707" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB707" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AC707" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD707" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE707" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF707" t="s" s="2">
+        <v>226</v>
+      </c>
+      <c r="AG707" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AH707" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AI707" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ707" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="AK707" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AL707" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AM707" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN707" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="s" s="2">
+        <v>1043</v>
+      </c>
+      <c r="B708" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="C708" s="2"/>
+      <c r="D708" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="E708" s="2"/>
+      <c r="F708" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G708" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="H708" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I708" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="J708" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="K708" t="s" s="2">
+        <v>150</v>
+      </c>
+      <c r="L708" t="s" s="2">
+        <v>231</v>
+      </c>
+      <c r="M708" t="s" s="2">
+        <v>232</v>
+      </c>
+      <c r="N708" s="2"/>
+      <c r="O708" s="2"/>
+      <c r="P708" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q708" s="2"/>
+      <c r="R708" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="S708" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="T708" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="U708" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="V708" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="W708" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X708" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Y708" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Z708" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AA708" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB708" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AC708" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD708" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE708" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF708" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="AG708" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH708" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AI708" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ708" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="AK708" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AL708" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AM708" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN708" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="s" s="2">
+        <v>1044</v>
+      </c>
+      <c r="B709" t="s" s="2">
+        <v>233</v>
+      </c>
+      <c r="C709" s="2"/>
+      <c r="D709" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="E709" s="2"/>
+      <c r="F709" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G709" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="H709" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I709" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="J709" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="K709" t="s" s="2">
+        <v>132</v>
+      </c>
+      <c r="L709" t="s" s="2">
+        <v>231</v>
+      </c>
+      <c r="M709" t="s" s="2">
+        <v>234</v>
+      </c>
+      <c r="N709" s="2"/>
+      <c r="O709" s="2"/>
+      <c r="P709" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q709" s="2"/>
+      <c r="R709" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="S709" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="T709" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="U709" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="V709" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="W709" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X709" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Y709" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Z709" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AA709" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB709" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AC709" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD709" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE709" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF709" t="s" s="2">
+        <v>233</v>
+      </c>
+      <c r="AG709" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH709" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AI709" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ709" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="AK709" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AL709" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AM709" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN709" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="s" s="2">
+        <v>1045</v>
+      </c>
+      <c r="B710" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="C710" s="2"/>
+      <c r="D710" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="E710" s="2"/>
+      <c r="F710" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G710" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="H710" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I710" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="J710" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="K710" t="s" s="2">
+        <v>150</v>
+      </c>
+      <c r="L710" t="s" s="2">
+        <v>236</v>
+      </c>
+      <c r="M710" t="s" s="2">
+        <v>237</v>
+      </c>
+      <c r="N710" s="2"/>
+      <c r="O710" s="2"/>
+      <c r="P710" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q710" s="2"/>
+      <c r="R710" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="S710" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="T710" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="U710" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="V710" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="W710" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X710" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Y710" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Z710" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AA710" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB710" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AC710" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD710" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE710" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF710" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="AG710" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH710" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AI710" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ710" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="AK710" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AL710" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AM710" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN710" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="s" s="2">
+        <v>1046</v>
+      </c>
+      <c r="B711" t="s" s="2">
+        <v>238</v>
+      </c>
+      <c r="C711" s="2"/>
+      <c r="D711" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="E711" s="2"/>
+      <c r="F711" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G711" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="H711" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I711" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="J711" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="K711" t="s" s="2">
+        <v>150</v>
+      </c>
+      <c r="L711" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="M711" t="s" s="2">
+        <v>240</v>
+      </c>
+      <c r="N711" s="2"/>
+      <c r="O711" s="2"/>
+      <c r="P711" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q711" s="2"/>
+      <c r="R711" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="S711" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="T711" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="U711" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="V711" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="W711" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X711" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Y711" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Z711" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AA711" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB711" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AC711" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD711" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE711" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF711" t="s" s="2">
+        <v>238</v>
+      </c>
+      <c r="AG711" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH711" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AI711" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ711" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="AK711" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AL711" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AM711" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN711" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="s" s="2">
+        <v>1047</v>
+      </c>
+      <c r="B712" t="s" s="2">
+        <v>241</v>
+      </c>
+      <c r="C712" s="2"/>
+      <c r="D712" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="E712" s="2"/>
+      <c r="F712" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G712" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="H712" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I712" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="J712" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="K712" t="s" s="2">
+        <v>145</v>
+      </c>
+      <c r="L712" t="s" s="2">
+        <v>242</v>
+      </c>
+      <c r="M712" t="s" s="2">
+        <v>243</v>
+      </c>
+      <c r="N712" s="2"/>
+      <c r="O712" s="2"/>
+      <c r="P712" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q712" s="2"/>
+      <c r="R712" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="S712" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="T712" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="U712" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="V712" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="W712" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X712" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Y712" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Z712" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AA712" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB712" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AC712" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD712" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE712" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF712" t="s" s="2">
+        <v>241</v>
+      </c>
+      <c r="AG712" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH712" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AI712" t="s" s="2">
+        <v>244</v>
+      </c>
+      <c r="AJ712" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="AK712" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AL712" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AM712" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN712" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="s" s="2">
+        <v>1048</v>
+      </c>
+      <c r="B713" t="s" s="2">
+        <v>245</v>
+      </c>
+      <c r="C713" s="2"/>
+      <c r="D713" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="E713" s="2"/>
+      <c r="F713" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G713" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="H713" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I713" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="J713" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="K713" t="s" s="2">
+        <v>150</v>
+      </c>
+      <c r="L713" t="s" s="2">
+        <v>151</v>
+      </c>
+      <c r="M713" t="s" s="2">
+        <v>152</v>
+      </c>
+      <c r="N713" s="2"/>
+      <c r="O713" s="2"/>
+      <c r="P713" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q713" s="2"/>
+      <c r="R713" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="S713" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="T713" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="U713" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="V713" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="W713" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X713" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Y713" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Z713" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AA713" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB713" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AC713" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD713" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE713" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF713" t="s" s="2">
+        <v>153</v>
+      </c>
+      <c r="AG713" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH713" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AI713" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ713" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AK713" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AL713" t="s" s="2">
+        <v>154</v>
+      </c>
+      <c r="AM713" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN713" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="s" s="2">
+        <v>1049</v>
+      </c>
+      <c r="B714" t="s" s="2">
+        <v>246</v>
+      </c>
+      <c r="C714" s="2"/>
+      <c r="D714" t="s" s="2">
+        <v>156</v>
+      </c>
+      <c r="E714" s="2"/>
+      <c r="F714" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G714" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="H714" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I714" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="J714" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="K714" t="s" s="2">
+        <v>157</v>
+      </c>
+      <c r="L714" t="s" s="2">
+        <v>158</v>
+      </c>
+      <c r="M714" t="s" s="2">
+        <v>159</v>
+      </c>
+      <c r="N714" t="s" s="2">
+        <v>160</v>
+      </c>
+      <c r="O714" s="2"/>
+      <c r="P714" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q714" s="2"/>
+      <c r="R714" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="S714" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="T714" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="U714" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="V714" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="W714" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X714" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Y714" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Z714" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AA714" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB714" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AC714" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD714" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE714" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF714" t="s" s="2">
+        <v>161</v>
+      </c>
+      <c r="AG714" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH714" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AI714" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ714" t="s" s="2">
+        <v>162</v>
+      </c>
+      <c r="AK714" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AL714" t="s" s="2">
+        <v>154</v>
+      </c>
+      <c r="AM714" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN714" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="s" s="2">
+        <v>1050</v>
+      </c>
+      <c r="B715" t="s" s="2">
+        <v>247</v>
+      </c>
+      <c r="C715" s="2"/>
+      <c r="D715" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="E715" s="2"/>
+      <c r="F715" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G715" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="H715" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I715" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="J715" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="K715" t="s" s="2">
+        <v>157</v>
+      </c>
+      <c r="L715" t="s" s="2">
+        <v>165</v>
+      </c>
+      <c r="M715" t="s" s="2">
+        <v>166</v>
+      </c>
+      <c r="N715" t="s" s="2">
+        <v>160</v>
+      </c>
+      <c r="O715" t="s" s="2">
+        <v>167</v>
+      </c>
+      <c r="P715" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q715" s="2"/>
+      <c r="R715" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="S715" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="T715" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="U715" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="V715" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="W715" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X715" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Y715" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Z715" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AA715" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB715" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AC715" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD715" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE715" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF715" t="s" s="2">
+        <v>168</v>
+      </c>
+      <c r="AG715" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH715" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AI715" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ715" t="s" s="2">
+        <v>162</v>
+      </c>
+      <c r="AK715" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AL715" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AM715" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN715" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="s" s="2">
+        <v>1051</v>
+      </c>
+      <c r="B716" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="C716" s="2"/>
+      <c r="D716" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="E716" s="2"/>
+      <c r="F716" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="G716" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="H716" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I716" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="J716" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="K716" t="s" s="2">
+        <v>150</v>
+      </c>
+      <c r="L716" t="s" s="2">
+        <v>249</v>
+      </c>
+      <c r="M716" t="s" s="2">
+        <v>250</v>
+      </c>
+      <c r="N716" s="2"/>
+      <c r="O716" s="2"/>
+      <c r="P716" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q716" s="2"/>
+      <c r="R716" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="S716" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="T716" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="U716" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="V716" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="W716" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X716" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Y716" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Z716" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AA716" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB716" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AC716" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD716" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE716" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF716" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="AG716" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AH716" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AI716" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ716" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="AK716" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AL716" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AM716" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN716" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="s" s="2">
+        <v>1052</v>
+      </c>
+      <c r="B717" t="s" s="2">
+        <v>251</v>
+      </c>
+      <c r="C717" s="2"/>
+      <c r="D717" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="E717" s="2"/>
+      <c r="F717" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G717" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="H717" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I717" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="J717" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="K717" t="s" s="2">
+        <v>101</v>
+      </c>
+      <c r="L717" t="s" s="2">
+        <v>252</v>
+      </c>
+      <c r="M717" t="s" s="2">
+        <v>253</v>
+      </c>
+      <c r="N717" s="2"/>
+      <c r="O717" s="2"/>
+      <c r="P717" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q717" s="2"/>
+      <c r="R717" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="S717" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="T717" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="U717" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="V717" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="W717" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X717" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Y717" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Z717" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AA717" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB717" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AC717" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD717" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE717" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF717" t="s" s="2">
+        <v>251</v>
+      </c>
+      <c r="AG717" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH717" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AI717" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ717" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="AK717" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AL717" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AM717" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN717" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="s" s="2">
+        <v>1053</v>
+      </c>
+      <c r="B718" t="s" s="2">
+        <v>254</v>
+      </c>
+      <c r="C718" s="2"/>
+      <c r="D718" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="E718" s="2"/>
+      <c r="F718" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G718" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="H718" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I718" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="J718" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="K718" t="s" s="2">
+        <v>150</v>
+      </c>
+      <c r="L718" t="s" s="2">
+        <v>255</v>
+      </c>
+      <c r="M718" t="s" s="2">
+        <v>256</v>
+      </c>
+      <c r="N718" t="s" s="2">
+        <v>257</v>
+      </c>
+      <c r="O718" s="2"/>
+      <c r="P718" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q718" s="2"/>
+      <c r="R718" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="S718" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="T718" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="U718" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="V718" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="W718" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X718" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Y718" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Z718" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AA718" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB718" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AC718" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD718" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE718" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF718" t="s" s="2">
+        <v>254</v>
+      </c>
+      <c r="AG718" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH718" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AI718" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ718" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="AK718" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AL718" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AM718" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN718" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="s" s="2">
+        <v>1054</v>
+      </c>
+      <c r="B719" t="s" s="2">
+        <v>258</v>
+      </c>
+      <c r="C719" s="2"/>
+      <c r="D719" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="E719" s="2"/>
+      <c r="F719" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G719" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="H719" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I719" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="J719" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="K719" t="s" s="2">
+        <v>132</v>
+      </c>
+      <c r="L719" t="s" s="2">
+        <v>259</v>
+      </c>
+      <c r="M719" t="s" s="2">
+        <v>260</v>
+      </c>
+      <c r="N719" t="s" s="2">
+        <v>261</v>
+      </c>
+      <c r="O719" s="2"/>
+      <c r="P719" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q719" s="2"/>
+      <c r="R719" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="S719" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="T719" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="U719" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="V719" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="W719" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X719" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Y719" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Z719" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AA719" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB719" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AC719" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD719" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE719" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF719" t="s" s="2">
+        <v>258</v>
+      </c>
+      <c r="AG719" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH719" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AI719" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ719" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="AK719" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AL719" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AM719" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN719" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="s" s="2">
+        <v>1055</v>
+      </c>
+      <c r="B720" t="s" s="2">
+        <v>262</v>
+      </c>
+      <c r="C720" s="2"/>
+      <c r="D720" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="E720" s="2"/>
+      <c r="F720" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G720" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="H720" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I720" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="J720" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="K720" t="s" s="2">
+        <v>193</v>
+      </c>
+      <c r="L720" t="s" s="2">
+        <v>263</v>
+      </c>
+      <c r="M720" t="s" s="2">
+        <v>264</v>
+      </c>
+      <c r="N720" t="s" s="2">
+        <v>265</v>
+      </c>
+      <c r="O720" s="2"/>
+      <c r="P720" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q720" s="2"/>
+      <c r="R720" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="S720" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="T720" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="U720" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="V720" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="W720" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X720" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Y720" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Z720" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AA720" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB720" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AC720" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD720" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE720" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF720" t="s" s="2">
+        <v>262</v>
+      </c>
+      <c r="AG720" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH720" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AI720" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ720" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AK720" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AL720" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AM720" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN720" t="s" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="s" s="2">
+        <v>1056</v>
+      </c>
+      <c r="B721" t="s" s="2">
+        <v>1056</v>
+      </c>
+      <c r="C721" s="2"/>
+      <c r="D721" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="E721" s="2"/>
+      <c r="F721" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G721" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="H721" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I721" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="J721" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="K721" t="s" s="2">
+        <v>1057</v>
+      </c>
+      <c r="L721" t="s" s="2">
+        <v>1058</v>
+      </c>
+      <c r="M721" t="s" s="2">
+        <v>1059</v>
+      </c>
+      <c r="N721" t="s" s="2">
+        <v>1060</v>
+      </c>
+      <c r="O721" t="s" s="2">
+        <v>1061</v>
+      </c>
+      <c r="P721" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Q721" s="2"/>
+      <c r="R721" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="S721" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="T721" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="U721" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="V721" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="W721" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="X721" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Y721" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="Z721" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AA721" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AB721" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AC721" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AD721" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AE721" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AF721" t="s" s="2">
+        <v>1056</v>
+      </c>
+      <c r="AG721" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH721" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AI721" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ721" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="AK721" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AL721" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AM721" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN721" t="s" s="2">
         <v>77</v>
       </c>
     </row>

</xml_diff>